<commit_message>
Up date the structure of batch processing files
</commit_message>
<xml_diff>
--- a/ClearMap/Scripts/Template/variable_file.xlsx
+++ b/ClearMap/Scripts/Template/variable_file.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stuberadmin\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stuberadmin\Desktop\SHIELD\ClearMap related files\ClearMap\ClearMap_ForHPC_UW\ClearMap\Scripts\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{654CBE8E-CBB6-42AC-ACD6-3EB134AAD2E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F597B38-509E-42B9-A956-2BC8CC5B70CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="752" firstSheet="1" activeTab="1" xr2:uid="{61B71D1B-A7AC-47B3-A961-00FCE0D70380}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="752" firstSheet="1" activeTab="7" xr2:uid="{61B71D1B-A7AC-47B3-A961-00FCE0D70380}"/>
   </bookViews>
   <sheets>
     <sheet name="thresholdParameter" sheetId="10" r:id="rId1"/>
@@ -69,9 +69,6 @@
     <t>processMethod</t>
   </si>
   <si>
-    <t>sequential</t>
-  </si>
-  <si>
     <t>PathReg</t>
   </si>
   <si>
@@ -96,9 +93,6 @@
     <t>method</t>
   </si>
   <si>
-    <t>classifier_path</t>
-  </si>
-  <si>
     <t>classindex</t>
   </si>
   <si>
@@ -214,6 +208,12 @@
   </si>
   <si>
     <t>(3,3,3)</t>
+  </si>
+  <si>
+    <t>parallel</t>
+  </si>
+  <si>
+    <t>classifier</t>
   </si>
 </sst>
 </file>
@@ -618,18 +618,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -641,50 +641,50 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCAD0F49-F2B1-4086-BF5B-BDC00B76680F}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -712,25 +712,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -750,7 +750,7 @@
         <v>100</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G2" s="3">
         <v>3</v>
@@ -794,7 +794,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -824,25 +824,25 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B2">
-        <v>250</v>
+        <v>50</v>
       </c>
       <c r="C2">
-        <v>200</v>
+        <v>25</v>
       </c>
       <c r="D2">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="E2" t="b">
         <v>0</v>
       </c>
       <c r="F2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>8</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -865,21 +865,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -892,22 +892,22 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N32" sqref="N32"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>56</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -922,134 +922,134 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06822A0D-C61A-464F-9B81-3D4B494EBE81}">
   <dimension ref="A1:Q3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P6" sqref="P6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>38</v>
-      </c>
       <c r="J1" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>34</v>
-      </c>
       <c r="F2" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="I2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="O2" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="J2" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>42</v>
-      </c>
       <c r="P2" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3" t="b">
         <v>1</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
@@ -1058,13 +1058,13 @@
         <v>1</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="O3" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="P3" s="3"/>
       <c r="Q3" s="3" t="b">

</xml_diff>

<commit_message>
Update the variable file
</commit_message>
<xml_diff>
--- a/ClearMap/Scripts/Template/variable_file.xlsx
+++ b/ClearMap/Scripts/Template/variable_file.xlsx
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stuberadmin\Desktop\SHIELD\ClearMap related files\ClearMap\ClearMap_ForHPC_UW\ClearMap\Scripts\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F597B38-509E-42B9-A956-2BC8CC5B70CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89D5701A-E37E-4DD2-A8D1-B9D878597E6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="752" firstSheet="1" activeTab="7" xr2:uid="{61B71D1B-A7AC-47B3-A961-00FCE0D70380}"/>
+    <workbookView xWindow="915" yWindow="2910" windowWidth="21855" windowHeight="11250" tabRatio="752" firstSheet="3" activeTab="5" xr2:uid="{61B71D1B-A7AC-47B3-A961-00FCE0D70380}"/>
   </bookViews>
   <sheets>
-    <sheet name="thresholdParameter" sheetId="10" r:id="rId1"/>
+    <sheet name="CropGeneratingParameter" sheetId="6" r:id="rId1"/>
     <sheet name="atlasParameter" sheetId="3" r:id="rId2"/>
-    <sheet name="CropGeneratingParameter" sheetId="6" r:id="rId3"/>
-    <sheet name="ResamplingParameter" sheetId="5" r:id="rId4"/>
-    <sheet name="StackProcessingParameter" sheetId="2" r:id="rId5"/>
-    <sheet name="voxelizeParameter" sheetId="7" r:id="rId6"/>
-    <sheet name="ilastikParameter" sheetId="4" r:id="rId7"/>
-    <sheet name="SpotDetectionParameter" sheetId="9" r:id="rId8"/>
+    <sheet name="ResamplingParameter" sheetId="5" r:id="rId3"/>
+    <sheet name="StackProcessingParameter" sheetId="2" r:id="rId4"/>
+    <sheet name="ilastikParameter" sheetId="4" r:id="rId5"/>
+    <sheet name="SpotDetectionParameter" sheetId="9" r:id="rId6"/>
+    <sheet name="thresholdParameter" sheetId="10" r:id="rId7"/>
+    <sheet name="voxelizeParameter" sheetId="7" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -150,15 +150,9 @@
     <t>removeBackgroundParameter</t>
   </si>
   <si>
-    <t>(4,4)</t>
-  </si>
-  <si>
     <t>filterDoGParameter</t>
   </si>
   <si>
-    <t>(6,6,11)</t>
-  </si>
-  <si>
     <t>sigma</t>
   </si>
   <si>
@@ -174,18 +168,12 @@
     <t>detectCellShapeParameter</t>
   </si>
   <si>
-    <t>(50,)</t>
-  </si>
-  <si>
     <t>ResolutionAffineSignalAutoFluo</t>
   </si>
   <si>
     <t>row</t>
   </si>
   <si>
-    <t>(15,300)</t>
-  </si>
-  <si>
     <t>(1,1)</t>
   </si>
   <si>
@@ -207,13 +195,25 @@
     <t>/PATH/TO/CLASSIFIER</t>
   </si>
   <si>
-    <t>(3,3,3)</t>
-  </si>
-  <si>
     <t>parallel</t>
   </si>
   <si>
     <t>classifier</t>
+  </si>
+  <si>
+    <t>(50,300)</t>
+  </si>
+  <si>
+    <t>(5,5)</t>
+  </si>
+  <si>
+    <t>(5,5,11)</t>
+  </si>
+  <si>
+    <t>(1,1,1)</t>
+  </si>
+  <si>
+    <t>(80,)</t>
   </si>
 </sst>
 </file>
@@ -604,98 +604,6 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69B38BFA-C54F-4506-8347-110F388BEA01}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="16384" width="9.140625" style="4"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCAD0F49-F2B1-4086-BF5B-BDC00B76680F}">
-  <dimension ref="A1:F3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="15" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B43DA83E-D86A-429D-9597-C6C832EFE925}">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -712,10 +620,10 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>20</v>
@@ -761,17 +669,74 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCAD0F49-F2B1-4086-BF5B-BDC00B76680F}">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="15" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CC8B472-CAF2-4A92-86FE-B83A2DA198D0}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="33.5703125" defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="33.5703125" style="2"/>
+    <col min="1" max="1" width="13.42578125" style="2" customWidth="1"/>
+    <col min="2" max="16384" width="33.5703125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -781,7 +746,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
-        <v>16</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -789,12 +754,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{079DC337-1068-4787-BF6B-7F3D33175770}">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -842,7 +807,7 @@
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -850,12 +815,239 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{287B4CFA-06E2-45C5-B387-32043016995B}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.140625" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06822A0D-C61A-464F-9B81-3D4B494EBE81}">
+  <dimension ref="A1:Q3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="13.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="O3" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69B38BFA-C54F-4506-8347-110F388BEA01}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E67A6EA5-D3B1-4B9F-89C4-B82ECAC3663C}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M25" sqref="M25"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -879,196 +1071,7 @@
         <v>26</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{287B4CFA-06E2-45C5-B387-32043016995B}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06822A0D-C61A-464F-9B81-3D4B494EBE81}">
-  <dimension ref="A1:Q3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="13.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="O3" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="P3" s="3"/>
-      <c r="Q3" s="3" t="b">
-        <v>1</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>